<commit_message>
working self create pin,updated Scanneractivity
</commit_message>
<xml_diff>
--- a/Hookpoints.xlsx
+++ b/Hookpoints.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Klasse</t>
   </si>
@@ -33,12 +27,6 @@
     <t>LoginActivity</t>
   </si>
   <si>
-    <t>Regel</t>
-  </si>
-  <si>
-    <t>Textlabel</t>
-  </si>
-  <si>
     <t>Onderdelen</t>
   </si>
   <si>
@@ -55,6 +43,123 @@
   </si>
   <si>
     <t>92, 97, 103</t>
+  </si>
+  <si>
+    <t>pincodeActivity</t>
+  </si>
+  <si>
+    <t>Innerklasse</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>checkPin</t>
+  </si>
+  <si>
+    <t>storedPin</t>
+  </si>
+  <si>
+    <t>30, 55, 79, 89</t>
+  </si>
+  <si>
+    <t>errorLabels</t>
+  </si>
+  <si>
+    <t>checkPin &amp; onComplete</t>
+  </si>
+  <si>
+    <t>64,83,92, 139,143</t>
+  </si>
+  <si>
+    <t>pinCreated</t>
+  </si>
+  <si>
+    <t>pin wordt opgeslagen(temp) en vergeleken met die van checkPin</t>
+  </si>
+  <si>
+    <t>Opnieuw ingevoerd na het maken van storedPin</t>
+  </si>
+  <si>
+    <t>Labels!</t>
+  </si>
+  <si>
+    <t>een controle of de pin is aangemaakt</t>
+  </si>
+  <si>
+    <t>Regel (gebruikt)</t>
+  </si>
+  <si>
+    <t>Als je de library wilt bestuderen: Pinlockview by Aritraroy</t>
+  </si>
+  <si>
+    <t>55, 62,81,137,154</t>
+  </si>
+  <si>
+    <t>ScannerActivity</t>
+  </si>
+  <si>
+    <t>fillInPass</t>
+  </si>
+  <si>
+    <t>dummyMail</t>
+  </si>
+  <si>
+    <t>loginText</t>
+  </si>
+  <si>
+    <t>submitButton</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>read&amp;Submit</t>
+  </si>
+  <si>
+    <t>Controle of de verifyCheck = true en doorsturen</t>
+  </si>
+  <si>
+    <t>verifyCheck</t>
+  </si>
+  <si>
+    <t>checkbox voor afvinken</t>
+  </si>
+  <si>
+    <t>73,98</t>
+  </si>
+  <si>
+    <t>StatusMessage</t>
+  </si>
+  <si>
+    <t>barcodeValue</t>
+  </si>
+  <si>
+    <t>informationValue</t>
+  </si>
+  <si>
+    <t>topLabel</t>
+  </si>
+  <si>
+    <t>secondBottomLabel</t>
+  </si>
+  <si>
+    <t>bottomLabel</t>
+  </si>
+  <si>
+    <t>labels!</t>
+  </si>
+  <si>
+    <t>Bij regel 136 is de conditie om een specifieke of een barcode te lezen</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137 t/m 144</t>
+  </si>
+  <si>
+    <t>146 t/m153</t>
   </si>
 </sst>
 </file>
@@ -90,10 +195,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,77 +490,285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>68.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>68.89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>66.87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="A22:B22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>